<commit_message>
Try Convert Feature Login
- edit name keyword > keywords
- add folder for test web
- add keyword for teardown login
- edit name capture screen shot
- add "sleep 2" to keyword Capture screen shot
- add localized
- add repository
- add test case (converted) 1-9
</commit_message>
<xml_diff>
--- a/Document/SCGP_QATraceBack/T1_SCGP_QATraceBack_TH_Test.xlsx
+++ b/Document/SCGP_QATraceBack/T1_SCGP_QATraceBack_TH_Test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -205,12 +205,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -304,13 +304,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -326,7 +326,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ชุดรูปแบบของ Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -400,7 +400,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -435,7 +434,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -611,25 +609,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.75" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="21.75" customWidth="1"/>
-    <col min="4" max="4" width="33.125" customWidth="1"/>
-    <col min="5" max="5" width="28.625" customWidth="1"/>
-    <col min="6" max="6" width="15.125" customWidth="1"/>
-    <col min="7" max="7" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="30.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -652,18 +650,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" ht="90">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -680,18 +678,20 @@
         <v>11</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="75">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
@@ -699,18 +699,20 @@
         <v>15</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="90">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
@@ -718,11 +720,11 @@
         <v>15</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="90">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -739,11 +741,11 @@
         <v>23</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="90">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -760,11 +762,11 @@
         <v>23</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="G7" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="90">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -781,11 +783,11 @@
         <v>32</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="90">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -802,11 +804,11 @@
         <v>47</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="90">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
@@ -823,11 +825,11 @@
         <v>46</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="90">
       <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
@@ -844,11 +846,11 @@
         <v>45</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -856,7 +858,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -864,7 +866,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -872,7 +874,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -880,7 +882,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -888,7 +890,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -896,7 +898,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -904,7 +906,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -912,7 +914,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -920,7 +922,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -928,7 +930,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -936,7 +938,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -944,7 +946,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -952,7 +954,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -960,7 +962,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -968,7 +970,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -976,7 +978,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -984,7 +986,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -992,7 +994,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1000,7 +1002,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1008,7 +1010,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1016,7 +1018,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1024,7 +1026,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1032,7 +1034,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1045,28 +1047,29 @@
     <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>